<commit_message>
convert string dates to datetime on excel download
</commit_message>
<xml_diff>
--- a/static/uploaded_data/output.xlsx
+++ b/static/uploaded_data/output.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,17 +429,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>40920</v>
       </c>
       <c r="D2" t="n">
         <v>28</v>
@@ -443,10 +443,8 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F2" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G2" t="n">
         <v>-0.2299794661190965</v>
@@ -471,17 +469,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Wed, 25 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>40933</v>
       </c>
       <c r="D3" t="n">
         <v>28</v>
@@ -489,10 +483,8 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F3" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G3" t="n">
         <v>-0.1943874058863792</v>
@@ -517,17 +509,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Thu, 26 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>40934</v>
       </c>
       <c r="D4" t="n">
         <v>28</v>
@@ -535,10 +523,8 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F4" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G4" t="n">
         <v>-0.1916495550992471</v>
@@ -563,17 +549,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Tue, 21 Feb 2012 00:00:00 GMT</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>40960</v>
       </c>
       <c r="D5" t="n">
         <v>28</v>
@@ -581,10 +563,8 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F5" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G5" t="n">
         <v>-0.1204654346338125</v>
@@ -609,17 +589,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Wed, 11 Apr 2012 00:00:00 GMT</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>41010</v>
       </c>
       <c r="D6" t="n">
         <v>28</v>
@@ -627,10 +603,8 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F6" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G6" t="n">
         <v>0.01642710472279261</v>
@@ -655,17 +629,13 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Thu, 10 Jan 2013 00:00:00 GMT</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>41284</v>
       </c>
       <c r="D7" t="n">
         <v>28</v>
@@ -673,10 +643,8 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F7" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G7" t="n">
         <v>0.7665982203969883</v>
@@ -701,17 +669,13 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Sat, 12 Jan 2013 00:00:00 GMT</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>41286</v>
       </c>
       <c r="D8" t="n">
         <v>28</v>
@@ -719,10 +683,8 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F8" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G8" t="n">
         <v>0.7720739219712526</v>
@@ -747,17 +709,13 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Fri, 10 Jan 2014 00:00:00 GMT</t>
-        </is>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>41649</v>
       </c>
       <c r="D9" t="n">
         <v>28</v>
@@ -765,10 +723,8 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F9" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G9" t="n">
         <v>1.765913757700205</v>
@@ -793,17 +749,13 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Sun, 12 Jan 2014 00:00:00 GMT</t>
-        </is>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>41651</v>
       </c>
       <c r="D10" t="n">
         <v>28</v>
@@ -811,10 +763,8 @@
       <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F10" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G10" t="n">
         <v>2.001368925393566</v>
@@ -839,17 +789,13 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Mon, 11 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>42380</v>
       </c>
       <c r="D11" t="n">
         <v>28</v>
@@ -857,10 +803,8 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F11" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G11" t="n">
         <v>3.997262149212868</v>
@@ -885,17 +829,13 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Wed, 13 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>42382</v>
       </c>
       <c r="D12" t="n">
         <v>28</v>
@@ -903,10 +843,8 @@
       <c r="E12" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Thu, 05 Apr 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F12" s="2" t="n">
+        <v>41004</v>
       </c>
       <c r="G12" t="n">
         <v>4.002737850787132</v>
@@ -931,17 +869,13 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>40920</v>
       </c>
       <c r="D13" t="n">
         <v>34</v>
@@ -949,10 +883,8 @@
       <c r="E13" t="n">
         <v>0</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F13" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G13" t="n">
         <v>-0.1149897330595483</v>
@@ -977,17 +909,13 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Wed, 25 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>40933</v>
       </c>
       <c r="D14" t="n">
         <v>34</v>
@@ -995,10 +923,8 @@
       <c r="E14" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F14" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G14" t="n">
         <v>-0.07939767282683094</v>
@@ -1023,17 +949,13 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Thu, 26 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>40934</v>
       </c>
       <c r="D15" t="n">
         <v>34</v>
@@ -1041,10 +963,8 @@
       <c r="E15" t="n">
         <v>0</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F15" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G15" t="n">
         <v>-0.07665982203969883</v>
@@ -1069,17 +989,13 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Tue, 21 Feb 2012 00:00:00 GMT</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>40960</v>
       </c>
       <c r="D16" t="n">
         <v>34</v>
@@ -1087,10 +1003,8 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F16" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G16" t="n">
         <v>-0.005475701574264203</v>
@@ -1115,17 +1029,13 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Wed, 13 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>41010</v>
       </c>
       <c r="D17" t="n">
         <v>34</v>
@@ -1133,16 +1043,14 @@
       <c r="E17" t="n">
         <v>0</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F17" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G17" t="n">
-        <v>4.002737850787132</v>
+        <v>0.1314168377823409</v>
       </c>
       <c r="H17" t="n">
-        <v>4.002737850787132</v>
+        <v>0.2464065708418891</v>
       </c>
       <c r="I17" t="n">
         <v>5</v>
@@ -1153,25 +1061,21 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>-13.41032932057559</v>
+        <v>-0.2262967931968165</v>
       </c>
       <c r="L17" t="n">
-        <v>2.630235665316258e-39</v>
+        <v>41.04852961824434</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Thu, 10 Jan 2013 00:00:00 GMT</t>
-        </is>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>41284</v>
       </c>
       <c r="D18" t="n">
         <v>34</v>
@@ -1179,10 +1083,8 @@
       <c r="E18" t="n">
         <v>0</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F18" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G18" t="n">
         <v>0.8815879534565366</v>
@@ -1207,17 +1109,13 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Sat, 12 Jan 2013 00:00:00 GMT</t>
-        </is>
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>41286</v>
       </c>
       <c r="D19" t="n">
         <v>34</v>
@@ -1225,10 +1123,8 @@
       <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F19" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G19" t="n">
         <v>1.002053388090349</v>
@@ -1253,17 +1149,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Fri, 10 Jan 2014 00:00:00 GMT</t>
-        </is>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>41649</v>
       </c>
       <c r="D20" t="n">
         <v>34</v>
@@ -1271,10 +1163,8 @@
       <c r="E20" t="n">
         <v>0</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F20" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G20" t="n">
         <v>1.995893223819302</v>
@@ -1299,17 +1189,13 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Sun, 12 Jan 2014 00:00:00 GMT</t>
-        </is>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>41651</v>
       </c>
       <c r="D21" t="n">
         <v>34</v>
@@ -1317,10 +1203,8 @@
       <c r="E21" t="n">
         <v>0</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F21" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G21" t="n">
         <v>2.001368925393566</v>
@@ -1345,17 +1229,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Mon, 11 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>42380</v>
       </c>
       <c r="D22" t="n">
         <v>34</v>
@@ -1363,10 +1243,8 @@
       <c r="E22" t="n">
         <v>0</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F22" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G22" t="n">
         <v>3.997262149212868</v>
@@ -1391,17 +1269,13 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Wed, 13 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>42382</v>
       </c>
       <c r="D23" t="n">
         <v>34</v>
@@ -1409,10 +1283,8 @@
       <c r="E23" t="n">
         <v>0</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Thu, 23 Feb 2012 00:00:00 GMT</t>
-        </is>
+      <c r="F23" s="2" t="n">
+        <v>40962</v>
       </c>
       <c r="G23" t="n">
         <v>4.002737850787132</v>
@@ -1437,17 +1309,13 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>40920</v>
       </c>
       <c r="D24" t="n">
         <v>39</v>
@@ -1479,17 +1347,13 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Wed, 25 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>40933</v>
       </c>
       <c r="D25" t="n">
         <v>39</v>
@@ -1521,17 +1385,13 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Thu, 26 Jan 2012 00:00:00 GMT</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>40934</v>
       </c>
       <c r="D26" t="n">
         <v>39</v>
@@ -1563,17 +1423,13 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Tue, 21 Feb 2012 00:00:00 GMT</t>
-        </is>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>40960</v>
       </c>
       <c r="D27" t="n">
         <v>39</v>
@@ -1605,17 +1461,13 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Wed, 13 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>41010</v>
       </c>
       <c r="D28" t="n">
         <v>39</v>
@@ -1625,10 +1477,10 @@
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
-        <v>4.002737850787132</v>
+        <v>0.2464065708418891</v>
       </c>
       <c r="H28" t="n">
-        <v>4.002737850787132</v>
+        <v>0.2464065708418891</v>
       </c>
       <c r="I28" t="n">
         <v>5</v>
@@ -1639,25 +1491,21 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>-13.41032932057559</v>
+        <v>-1.987173240679111</v>
       </c>
       <c r="L28" t="n">
-        <v>2.630235665316258e-39</v>
+        <v>2.34516010760982</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Thu, 10 Jan 2013 00:00:00 GMT</t>
-        </is>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>41284</v>
       </c>
       <c r="D29" t="n">
         <v>39</v>
@@ -1689,17 +1537,13 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Sat, 12 Jan 2013 00:00:00 GMT</t>
-        </is>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>41286</v>
       </c>
       <c r="D30" t="n">
         <v>39</v>
@@ -1731,17 +1575,13 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Fri, 10 Jan 2014 00:00:00 GMT</t>
-        </is>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>41649</v>
       </c>
       <c r="D31" t="n">
         <v>39</v>
@@ -1773,17 +1613,13 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Sun, 12 Jan 2014 00:00:00 GMT</t>
-        </is>
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>41651</v>
       </c>
       <c r="D32" t="n">
         <v>39</v>
@@ -1815,17 +1651,13 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Mon, 11 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>42380</v>
       </c>
       <c r="D33" t="n">
         <v>39</v>
@@ -1857,17 +1689,13 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Thu, 12 Jan 2012 00:00:00 GMT</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Wed, 13 Jan 2016 00:00:00 GMT</t>
-        </is>
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>40920</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>42382</v>
       </c>
       <c r="D34" t="n">
         <v>39</v>

</xml_diff>